<commit_message>
Making progress on dropdown code generator
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IsaiahMartin\source\repos\CalcPad Testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IsaiahMartin\source\repos\CalcpadGenerator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{F54E8CDC-DA01-4975-B892-3D1DC684F582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7262EDA8-1F49-4316-9266-01399279BEF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11175" xr2:uid="{A45A5AA5-646A-468D-A059-024355DA9CB2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{A45A5AA5-646A-468D-A059-024355DA9CB2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,6 @@
     <definedName name="Test_Defined_Name">Sheet1!$B$10:$D$12</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
   <si>
     <t>Test Table</t>
   </si>
@@ -74,6 +73,21 @@
   </si>
   <si>
     <t>mm</t>
+  </si>
+  <si>
+    <t>hi</t>
+  </si>
+  <si>
+    <t>hello</t>
+  </si>
+  <si>
+    <t>rawr</t>
+  </si>
+  <si>
+    <t>v1</t>
+  </si>
+  <si>
+    <t>v2</t>
   </si>
 </sst>
 </file>
@@ -473,7 +487,7 @@
   <dimension ref="A2:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,13 +503,13 @@
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="J2" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -508,8 +522,8 @@
       <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="I3">
-        <v>1</v>
+      <c r="I3" t="s">
+        <v>12</v>
       </c>
       <c r="J3">
         <v>2</v>
@@ -528,8 +542,8 @@
       <c r="D4">
         <v>3</v>
       </c>
-      <c r="I4">
-        <v>4.5</v>
+      <c r="I4" t="s">
+        <v>13</v>
       </c>
       <c r="J4">
         <v>6.7</v>
@@ -548,8 +562,8 @@
       <c r="D5">
         <v>8.9</v>
       </c>
-      <c r="I5">
-        <v>400</v>
+      <c r="I5" t="s">
+        <v>11</v>
       </c>
       <c r="J5">
         <v>4000000000000</v>

</xml_diff>